<commit_message>
added new plots and deleted old plots
</commit_message>
<xml_diff>
--- a/transcriptome_genome_annotation/plots/geoduck_tables.xlsx
+++ b/transcriptome_genome_annotation/plots/geoduck_tables.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviacattau/Documents/GitHub/code-for-Pgenerosa/transcriptome_genome_annotation/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8119AA5A-FA41-8D42-9BB3-306619C76B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AD37B2-E253-C041-8660-5435CEFAC116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="500" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{4342BFFC-51E7-954C-9082-9528990B46CD}"/>
+    <workbookView xWindow="-30520" yWindow="-1000" windowWidth="27640" windowHeight="16440" activeTab="6" xr2:uid="{4342BFFC-51E7-954C-9082-9528990B46CD}"/>
   </bookViews>
   <sheets>
-    <sheet name="blast hits" sheetId="4" r:id="rId1"/>
-    <sheet name="single tissue" sheetId="1" r:id="rId2"/>
-    <sheet name="Dheilly genes" sheetId="20" r:id="rId3"/>
-    <sheet name="differnetially expressed specie" sheetId="19" r:id="rId4"/>
-    <sheet name="GOterms transcriptome  normal" sheetId="12" r:id="rId5"/>
-    <sheet name="overlapping" sheetId="3" r:id="rId6"/>
+    <sheet name="overlapping" sheetId="3" r:id="rId1"/>
+    <sheet name="blast hits" sheetId="4" r:id="rId2"/>
+    <sheet name="single tissue" sheetId="1" r:id="rId3"/>
+    <sheet name="Dheilly genes" sheetId="20" r:id="rId4"/>
+    <sheet name="differnetially expressed specie" sheetId="19" r:id="rId5"/>
+    <sheet name="GOterms transcriptome  normal" sheetId="12" r:id="rId6"/>
     <sheet name="Top20 tissue unique" sheetId="17" r:id="rId7"/>
     <sheet name="go terms for discussion" sheetId="18" r:id="rId8"/>
     <sheet name="total genes with hits tissues" sheetId="11" r:id="rId9"/>
@@ -35,7 +35,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'% found in tissue'!$A$1:$D$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'GOterms transcriptome  normal'!$M$1:$O$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'GOterms transcriptome  normal'!$M$1:$O$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'top 20 terms species'!$A$1:$A$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'top 20 tissue unique'!$A$1:$A$251</definedName>
   </definedNames>
@@ -1660,578 +1660,479 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7B8103-F7E6-ED47-8F23-029A359B5999}">
-  <dimension ref="A1:K28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497FF3B9-83D1-4847-A17F-7F4FA7D8EA43}">
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>183</v>
+        <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2">
+        <v>1974</v>
+      </c>
+      <c r="J2">
+        <v>65</v>
+      </c>
+      <c r="K2">
+        <v>60</v>
+      </c>
+      <c r="L2" s="16">
+        <f>J2/I2</f>
+        <v>3.292806484295846E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="4">
+        <v>101</v>
+      </c>
+      <c r="G3" s="4">
+        <v>665</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4">
+        <v>665</v>
+      </c>
+      <c r="J3" s="4">
+        <v>46</v>
+      </c>
+      <c r="K3" s="4">
+        <v>54</v>
+      </c>
+      <c r="L3" s="16">
+        <f t="shared" ref="L3:L11" si="0">J3/I3</f>
+        <v>6.9172932330827067E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="4">
+        <v>10001</v>
+      </c>
+      <c r="G4" s="4">
+        <v>545</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="4">
+        <v>545</v>
+      </c>
+      <c r="J4" s="4">
+        <v>49</v>
+      </c>
+      <c r="K4" s="4">
+        <v>55</v>
+      </c>
+      <c r="L4" s="16">
+        <f t="shared" si="0"/>
+        <v>8.990825688073395E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1001</v>
+      </c>
+      <c r="G5" s="4">
+        <v>155</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="4">
+        <v>155</v>
+      </c>
+      <c r="J5" s="4">
+        <v>35</v>
+      </c>
+      <c r="K5" s="4">
         <v>41</v>
       </c>
-      <c r="C2" s="44">
-        <v>5099</v>
-      </c>
-      <c r="D2" s="44">
-        <v>2198</v>
-      </c>
-      <c r="E2" s="44">
-        <v>980</v>
-      </c>
-      <c r="H2" s="48" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="44">
-        <v>657</v>
-      </c>
-      <c r="D3" s="44">
-        <v>1235</v>
-      </c>
-      <c r="E3" s="44">
-        <v>210</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="45" t="s">
+      <c r="L5" s="16">
+        <f t="shared" si="0"/>
+        <v>0.22580645161290322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10100</v>
+      </c>
+      <c r="G6" s="4">
+        <v>124</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="4">
+        <v>124</v>
+      </c>
+      <c r="J6" s="4">
+        <v>18</v>
+      </c>
+      <c r="K6" s="4">
+        <v>25</v>
+      </c>
+      <c r="L6" s="16">
+        <f t="shared" si="0"/>
+        <v>0.14516129032258066</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4">
+        <v>110</v>
+      </c>
+      <c r="G7" s="4">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="4">
+        <v>79</v>
+      </c>
+      <c r="J7" s="4">
+        <v>20</v>
+      </c>
+      <c r="K7" s="4">
+        <v>28</v>
+      </c>
+      <c r="L7" s="16">
+        <f t="shared" si="0"/>
+        <v>0.25316455696202533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4">
+        <v>10010</v>
+      </c>
+      <c r="G8" s="4">
+        <v>60</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="4">
+        <v>60</v>
+      </c>
+      <c r="J8" s="4">
+        <v>13</v>
+      </c>
+      <c r="K8" s="4">
+        <v>17</v>
+      </c>
+      <c r="L8" s="16">
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1010</v>
+      </c>
+      <c r="G9" s="4">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="4">
+        <v>46</v>
+      </c>
+      <c r="J9" s="4">
+        <v>4</v>
+      </c>
+      <c r="K9" s="4">
+        <v>22</v>
+      </c>
+      <c r="L9" s="16">
+        <f t="shared" si="0"/>
+        <v>8.6956521739130432E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4">
+        <v>11000</v>
+      </c>
+      <c r="G10" s="4">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="4">
+        <v>43</v>
+      </c>
+      <c r="J10" s="4">
+        <v>11</v>
+      </c>
+      <c r="K10" s="4">
+        <v>17</v>
+      </c>
+      <c r="L10" s="16">
+        <f t="shared" si="0"/>
+        <v>0.2558139534883721</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1100</v>
+      </c>
+      <c r="G11" s="4">
+        <v>20</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="4">
+        <v>20</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+      <c r="K11" s="4">
+        <v>6</v>
+      </c>
+      <c r="L11" s="16">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="I12" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>10000</v>
+      </c>
+      <c r="G13">
+        <v>371</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13">
+        <v>371</v>
+      </c>
+      <c r="K13" s="4">
         <v>41</v>
       </c>
-      <c r="B4" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="45">
-        <v>6521</v>
-      </c>
-      <c r="D4" s="45">
-        <v>7027</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="H4" s="48" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="45">
-        <v>761</v>
-      </c>
-      <c r="D5" s="45">
-        <v>1390</v>
-      </c>
-      <c r="E5" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="47">
-        <v>34947</v>
-      </c>
-      <c r="D6" s="47">
-        <v>17611</v>
-      </c>
-      <c r="E6" s="46">
-        <v>1029</v>
-      </c>
-      <c r="H6" s="48" t="s">
-        <v>227</v>
-      </c>
-      <c r="J6" s="48"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="H7" s="48"/>
-      <c r="J7" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="H8" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="I8">
-        <v>761</v>
-      </c>
-      <c r="J8" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="K8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="B9" t="s">
-        <v>229</v>
-      </c>
-      <c r="C9">
-        <v>8736</v>
-      </c>
-      <c r="D9">
-        <v>271</v>
-      </c>
-      <c r="E9" t="s">
-        <v>221</v>
-      </c>
-      <c r="H9" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="I9">
-        <v>6521</v>
-      </c>
-      <c r="J9" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="K9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="48" t="s">
-        <v>224</v>
-      </c>
-      <c r="B10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C10">
-        <v>874</v>
-      </c>
-      <c r="D10">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>221</v>
-      </c>
-      <c r="H10" s="48" t="s">
-        <v>238</v>
-      </c>
-      <c r="I10">
-        <v>657</v>
-      </c>
-      <c r="J10" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11" t="s">
-        <v>229</v>
-      </c>
-      <c r="C11">
-        <v>2263</v>
-      </c>
-      <c r="D11">
-        <v>994</v>
-      </c>
-      <c r="E11" t="s">
-        <v>222</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="I11">
-        <v>5099</v>
-      </c>
-      <c r="J11" s="48" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12" t="s">
-        <v>229</v>
-      </c>
-      <c r="C12">
-        <v>3268</v>
-      </c>
-      <c r="D12">
-        <v>61</v>
-      </c>
-      <c r="E12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="48" t="s">
-        <v>227</v>
-      </c>
-      <c r="B13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13">
-        <v>1629</v>
-      </c>
-      <c r="D13">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="49" t="s">
-        <v>219</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="B16" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16">
-        <v>5099</v>
-      </c>
-      <c r="D16">
-        <v>210</v>
-      </c>
-      <c r="E16" t="s">
-        <v>221</v>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14">
+        <v>1000</v>
+      </c>
+      <c r="G14">
+        <v>119</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14">
+        <v>119</v>
+      </c>
+      <c r="J14" s="4">
+        <v>7</v>
+      </c>
+      <c r="K14" s="4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>340</v>
+      </c>
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15">
+        <v>340</v>
+      </c>
+      <c r="K15" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16">
+        <v>868</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="I16">
-        <v>1235</v>
-      </c>
-      <c r="J16">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>229</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17">
-        <v>6521</v>
-      </c>
-      <c r="D17" t="s">
-        <v>164</v>
-      </c>
+        <v>868</v>
+      </c>
+      <c r="K16">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="E17" t="s">
-        <v>221</v>
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2180</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="I17">
-        <v>1390</v>
-      </c>
-      <c r="J17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="B18" t="s">
-        <v>229</v>
-      </c>
-      <c r="C18">
-        <v>657</v>
-      </c>
-      <c r="D18">
-        <v>980</v>
-      </c>
-      <c r="E18" t="s">
-        <v>222</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18">
-        <v>2198</v>
-      </c>
-      <c r="J18">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>229</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="C19">
-        <v>761</v>
-      </c>
-      <c r="D19" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" t="s">
-        <v>222</v>
-      </c>
-      <c r="H19" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19">
-        <v>7027</v>
-      </c>
-      <c r="J19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>229</v>
-      </c>
-      <c r="B20" t="s">
-        <v>230</v>
-      </c>
-      <c r="C20" s="8">
-        <v>34947</v>
-      </c>
-      <c r="D20">
-        <v>1029</v>
-      </c>
-      <c r="E20" t="s">
-        <v>221</v>
-      </c>
-      <c r="H20" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20">
-        <v>17611</v>
-      </c>
-      <c r="J20">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>229</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="C23">
-        <v>980</v>
-      </c>
-      <c r="D23">
-        <v>778</v>
-      </c>
-      <c r="E23">
-        <v>68</v>
-      </c>
-      <c r="H23" t="s">
-        <v>171</v>
-      </c>
-      <c r="I23">
-        <v>778</v>
-      </c>
-      <c r="J23">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" t="s">
-        <v>229</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>225</v>
-      </c>
-      <c r="C24">
-        <v>210</v>
-      </c>
-      <c r="D24">
-        <v>8</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
-      <c r="H24" t="s">
-        <v>172</v>
-      </c>
-      <c r="I24">
-        <v>8</v>
-      </c>
-      <c r="J24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="50" t="s">
-        <v>225</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>223</v>
-      </c>
-      <c r="C25">
-        <v>202</v>
-      </c>
-      <c r="D25">
-        <v>202</v>
-      </c>
-      <c r="E25">
-        <v>54</v>
-      </c>
-      <c r="H25" t="s">
-        <v>173</v>
-      </c>
-      <c r="I25">
-        <v>202</v>
-      </c>
-      <c r="J25">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="H26" t="s">
-        <v>174</v>
-      </c>
-      <c r="I26">
-        <v>41</v>
-      </c>
-      <c r="J26">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="H28" t="s">
-        <v>185</v>
-      </c>
+        <v>2180</v>
+      </c>
+      <c r="K17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G12">
+    <sortCondition descending="1" ref="G1:G12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3985,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4767766-F7E2-344D-9E33-FADFFD2065BE}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4040,10 +3941,10 @@
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4066,10 +3967,10 @@
       <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4092,10 +3993,10 @@
       <c r="G4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4118,10 +4019,10 @@
       <c r="G5" t="s">
         <v>46</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>56</v>
       </c>
     </row>
@@ -4144,10 +4045,10 @@
       <c r="G6" t="s">
         <v>47</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4170,10 +4071,10 @@
       <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4196,10 +4097,10 @@
       <c r="G8" t="s">
         <v>56</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4222,10 +4123,10 @@
       <c r="G9" t="s">
         <v>52</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4248,10 +4149,10 @@
       <c r="G10" t="s">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4274,10 +4175,10 @@
       <c r="G11" t="s">
         <v>55</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -9797,7 +9698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20026194-68BA-8C44-8F05-04AF419EA4FD}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -11497,7 +11398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22A8816-EA9A-1545-B9C3-92E9C4A43359}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -12826,11 +12727,589 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7B8103-F7E6-ED47-8F23-029A359B5999}">
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="44">
+        <v>5099</v>
+      </c>
+      <c r="D2" s="44">
+        <v>2198</v>
+      </c>
+      <c r="E2" s="44">
+        <v>980</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="44">
+        <v>657</v>
+      </c>
+      <c r="D3" s="44">
+        <v>1235</v>
+      </c>
+      <c r="E3" s="44">
+        <v>210</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="45">
+        <v>6521</v>
+      </c>
+      <c r="D4" s="45">
+        <v>7027</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="H4" s="48" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="45">
+        <v>761</v>
+      </c>
+      <c r="D5" s="45">
+        <v>1390</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="48" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="47">
+        <v>34947</v>
+      </c>
+      <c r="D6" s="47">
+        <v>17611</v>
+      </c>
+      <c r="E6" s="46">
+        <v>1029</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="J6" s="48"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="H7" s="48"/>
+      <c r="J7" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="I8">
+        <v>761</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="K8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9">
+        <v>8736</v>
+      </c>
+      <c r="D9">
+        <v>271</v>
+      </c>
+      <c r="E9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="I9">
+        <v>6521</v>
+      </c>
+      <c r="J9" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="K9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10">
+        <v>874</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>221</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="I10">
+        <v>657</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C11">
+        <v>2263</v>
+      </c>
+      <c r="D11">
+        <v>994</v>
+      </c>
+      <c r="E11" t="s">
+        <v>222</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>239</v>
+      </c>
+      <c r="I11">
+        <v>5099</v>
+      </c>
+      <c r="J11" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12" t="s">
+        <v>229</v>
+      </c>
+      <c r="C12">
+        <v>3268</v>
+      </c>
+      <c r="D12">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" t="s">
+        <v>229</v>
+      </c>
+      <c r="C13">
+        <v>1629</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="49" t="s">
+        <v>219</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16">
+        <v>5099</v>
+      </c>
+      <c r="D16">
+        <v>210</v>
+      </c>
+      <c r="E16" t="s">
+        <v>221</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16">
+        <v>1235</v>
+      </c>
+      <c r="J16">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17">
+        <v>6521</v>
+      </c>
+      <c r="D17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" t="s">
+        <v>221</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17">
+        <v>1390</v>
+      </c>
+      <c r="J17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="B18" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18">
+        <v>657</v>
+      </c>
+      <c r="D18">
+        <v>980</v>
+      </c>
+      <c r="E18" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18">
+        <v>2198</v>
+      </c>
+      <c r="J18">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>229</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19">
+        <v>761</v>
+      </c>
+      <c r="D19" t="s">
+        <v>164</v>
+      </c>
+      <c r="E19" t="s">
+        <v>222</v>
+      </c>
+      <c r="H19" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19">
+        <v>7027</v>
+      </c>
+      <c r="J19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="8">
+        <v>34947</v>
+      </c>
+      <c r="D20">
+        <v>1029</v>
+      </c>
+      <c r="E20" t="s">
+        <v>221</v>
+      </c>
+      <c r="H20" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20">
+        <v>17611</v>
+      </c>
+      <c r="J20">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23">
+        <v>980</v>
+      </c>
+      <c r="D23">
+        <v>778</v>
+      </c>
+      <c r="E23">
+        <v>68</v>
+      </c>
+      <c r="H23" t="s">
+        <v>171</v>
+      </c>
+      <c r="I23">
+        <v>778</v>
+      </c>
+      <c r="J23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="C24">
+        <v>210</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24">
+        <v>8</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25">
+        <v>202</v>
+      </c>
+      <c r="D25">
+        <v>202</v>
+      </c>
+      <c r="E25">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25">
+        <v>202</v>
+      </c>
+      <c r="J25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="H26" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26">
+        <v>41</v>
+      </c>
+      <c r="J26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="H28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FBD0D9-15F7-B440-A087-0EA0AA5080F3}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13151,12 +13630,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980BDE0C-572B-464B-9775-865EEF875FC1}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -13360,7 +13839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD928342-7831-7641-B92C-498582038E8A}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -13519,11 +13998,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FB9069-9636-FA4A-B89A-564862881889}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
@@ -14249,491 +14728,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497FF3B9-83D1-4847-A17F-7F4FA7D8EA43}">
-  <dimension ref="A1:M19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2">
-        <v>1974</v>
-      </c>
-      <c r="J2">
-        <v>65</v>
-      </c>
-      <c r="K2">
-        <v>60</v>
-      </c>
-      <c r="L2" s="16">
-        <f>J2/I2</f>
-        <v>3.292806484295846E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4">
-        <v>101</v>
-      </c>
-      <c r="G3" s="4">
-        <v>665</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="4">
-        <v>665</v>
-      </c>
-      <c r="J3" s="4">
-        <v>46</v>
-      </c>
-      <c r="K3" s="4">
-        <v>54</v>
-      </c>
-      <c r="L3" s="16">
-        <f t="shared" ref="L3:L11" si="0">J3/I3</f>
-        <v>6.9172932330827067E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="4">
-        <v>10001</v>
-      </c>
-      <c r="G4" s="4">
-        <v>545</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="4">
-        <v>545</v>
-      </c>
-      <c r="J4" s="4">
-        <v>49</v>
-      </c>
-      <c r="K4" s="4">
-        <v>55</v>
-      </c>
-      <c r="L4" s="16">
-        <f t="shared" si="0"/>
-        <v>8.990825688073395E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1001</v>
-      </c>
-      <c r="G5" s="4">
-        <v>155</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="4">
-        <v>155</v>
-      </c>
-      <c r="J5" s="4">
-        <v>35</v>
-      </c>
-      <c r="K5" s="4">
-        <v>41</v>
-      </c>
-      <c r="L5" s="16">
-        <f t="shared" si="0"/>
-        <v>0.22580645161290322</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4">
-        <v>10100</v>
-      </c>
-      <c r="G6" s="4">
-        <v>124</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="4">
-        <v>124</v>
-      </c>
-      <c r="J6" s="4">
-        <v>18</v>
-      </c>
-      <c r="K6" s="4">
-        <v>25</v>
-      </c>
-      <c r="L6" s="16">
-        <f t="shared" si="0"/>
-        <v>0.14516129032258066</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="4">
-        <v>110</v>
-      </c>
-      <c r="G7" s="4">
-        <v>79</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="4">
-        <v>79</v>
-      </c>
-      <c r="J7" s="4">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4">
-        <v>28</v>
-      </c>
-      <c r="L7" s="16">
-        <f t="shared" si="0"/>
-        <v>0.25316455696202533</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4">
-        <v>10010</v>
-      </c>
-      <c r="G8" s="4">
-        <v>60</v>
-      </c>
-      <c r="H8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="4">
-        <v>60</v>
-      </c>
-      <c r="J8" s="4">
-        <v>13</v>
-      </c>
-      <c r="K8" s="4">
-        <v>17</v>
-      </c>
-      <c r="L8" s="16">
-        <f t="shared" si="0"/>
-        <v>0.21666666666666667</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1010</v>
-      </c>
-      <c r="G9" s="4">
-        <v>46</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="4">
-        <v>46</v>
-      </c>
-      <c r="J9" s="4">
-        <v>4</v>
-      </c>
-      <c r="K9" s="4">
-        <v>22</v>
-      </c>
-      <c r="L9" s="16">
-        <f t="shared" si="0"/>
-        <v>8.6956521739130432E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="4">
-        <v>11000</v>
-      </c>
-      <c r="G10" s="4">
-        <v>43</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="4">
-        <v>43</v>
-      </c>
-      <c r="J10" s="4">
-        <v>11</v>
-      </c>
-      <c r="K10" s="4">
-        <v>17</v>
-      </c>
-      <c r="L10" s="16">
-        <f t="shared" si="0"/>
-        <v>0.2558139534883721</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1100</v>
-      </c>
-      <c r="G11" s="4">
-        <v>20</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="4">
-        <v>20</v>
-      </c>
-      <c r="J11" s="4">
-        <v>1</v>
-      </c>
-      <c r="K11" s="4">
-        <v>6</v>
-      </c>
-      <c r="L11" s="16">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="I12" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <v>10000</v>
-      </c>
-      <c r="G13">
-        <v>371</v>
-      </c>
-      <c r="H13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13">
-        <v>371</v>
-      </c>
-      <c r="K13" s="4">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14">
-        <v>1000</v>
-      </c>
-      <c r="G14">
-        <v>119</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14">
-        <v>119</v>
-      </c>
-      <c r="J14" s="4">
-        <v>7</v>
-      </c>
-      <c r="K14" s="4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15">
-        <v>100</v>
-      </c>
-      <c r="G15">
-        <v>340</v>
-      </c>
-      <c r="H15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15">
-        <v>340</v>
-      </c>
-      <c r="K15" s="4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16">
-        <v>10</v>
-      </c>
-      <c r="G16">
-        <v>868</v>
-      </c>
-      <c r="H16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16">
-        <v>868</v>
-      </c>
-      <c r="K16">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>2180</v>
-      </c>
-      <c r="H17" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17">
-        <v>2180</v>
-      </c>
-      <c r="K17">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G12">
-    <sortCondition descending="1" ref="G1:G12"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8E42923-874F-0942-A327-3143864B57A6}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>